<commit_message>
WIP on fixing camera transformations.
</commit_message>
<xml_diff>
--- a/data/01_raw/2023_ground_truth_counts.xlsx
+++ b/data/01_raw/2023_ground_truth_counts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawest\OneDrive - University of Georgia\Documents\UGA Grad School\Masters Research\PTs Drone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/dawest_uga_edu/Documents/Documents/UGA Grad School/Masters Research/PTs Drone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB10389E-1E38-42AC-BD75-6DAE21E95AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABA7B3B8-0205-42DC-9FC6-46E91AAE057E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="8" activeTab="8" xr2:uid="{8F9DACAF-C196-4FF0-BBE7-23C747EA27F6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="9" activeTab="9" xr2:uid="{8F9DACAF-C196-4FF0-BBE7-23C747EA27F6}"/>
   </bookViews>
   <sheets>
     <sheet name="7-27-23" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="8-18-23" sheetId="7" r:id="rId7"/>
     <sheet name="8-21-23" sheetId="8" r:id="rId8"/>
     <sheet name="8-24-23" sheetId="9" r:id="rId9"/>
+    <sheet name="8-28-23" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="13">
   <si>
     <t>Plot</t>
   </si>
@@ -1062,6 +1063,715 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D46B11-767A-489E-8D54-D89AFE4819EB}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="8" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="19.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>45166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="2">
+        <v>1006</v>
+      </c>
+      <c r="B2" s="2">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="2">
+        <v>1010</v>
+      </c>
+      <c r="B3" s="2">
+        <v>58</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="2">
+        <v>1074</v>
+      </c>
+      <c r="B4" s="2">
+        <v>74</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="2">
+        <v>1078</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="2">
+        <v>1093</v>
+      </c>
+      <c r="B6" s="2">
+        <v>66</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="2">
+        <v>1095</v>
+      </c>
+      <c r="B7" s="2">
+        <v>128</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="2">
+        <v>1098</v>
+      </c>
+      <c r="B8" s="2">
+        <v>191</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="2">
+        <v>1132</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="2">
+        <v>1142</v>
+      </c>
+      <c r="B10" s="2">
+        <v>207</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="2">
+        <v>1147</v>
+      </c>
+      <c r="B11" s="2">
+        <v>40</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="2">
+        <v>1150</v>
+      </c>
+      <c r="B12" s="2">
+        <v>202</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="2">
+        <v>1156</v>
+      </c>
+      <c r="B13" s="2">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>9</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="2">
+        <v>1261</v>
+      </c>
+      <c r="B14" s="2">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="2">
+        <v>1263</v>
+      </c>
+      <c r="B15" s="2">
+        <v>202</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="2">
+        <v>1334</v>
+      </c>
+      <c r="B16" s="2">
+        <v>191</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="2">
+        <v>1371</v>
+      </c>
+      <c r="B17" s="2">
+        <v>207</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2">
+        <v>13</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="2">
+        <v>1376</v>
+      </c>
+      <c r="B18" s="2">
+        <v>62</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2">
+        <v>10</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="2">
+        <v>1382</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>8</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="2">
+        <v>1406</v>
+      </c>
+      <c r="B20" s="2">
+        <v>74</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>8</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="2">
+        <v>1459</v>
+      </c>
+      <c r="B21" s="2">
+        <v>128</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2">
+        <v>12</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="2">
+        <v>1485</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>12</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="2">
+        <v>1489</v>
+      </c>
+      <c r="B23" s="2">
+        <v>58</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="2">
+        <v>1493</v>
+      </c>
+      <c r="B24" s="2">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="2">
+        <v>1513</v>
+      </c>
+      <c r="B25" s="2">
+        <v>66</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>8</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A26" s="2">
+        <v>1528</v>
+      </c>
+      <c r="B26" s="2">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A27" s="2">
+        <v>1529</v>
+      </c>
+      <c r="B27" s="2">
+        <v>202</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>11</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="2">
+        <v>1536</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="2">
+        <v>1564</v>
+      </c>
+      <c r="B29" s="2">
+        <v>62</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>14</v>
+      </c>
+      <c r="E29" s="2">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A30" s="2">
+        <v>1606</v>
+      </c>
+      <c r="B30" s="2">
+        <v>58</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+      <c r="D30" s="2">
+        <v>6</v>
+      </c>
+      <c r="E30" s="2">
+        <v>14</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="2">
+        <v>1642</v>
+      </c>
+      <c r="B31" s="2">
+        <v>207</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
+      <c r="D31" s="2">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2">
+        <v>7</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="2">
+        <v>1646</v>
+      </c>
+      <c r="B32" s="2">
+        <v>74</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="2">
+        <v>11</v>
+      </c>
+      <c r="E32" s="2">
+        <v>16</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="2">
+        <v>1676</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2">
+        <v>7</v>
+      </c>
+      <c r="E33" s="2">
+        <v>13</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="2">
+        <v>1682</v>
+      </c>
+      <c r="B34" s="2">
+        <v>128</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2">
+        <v>10</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A35" s="2">
+        <v>1688</v>
+      </c>
+      <c r="B35" s="2">
+        <v>66</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>6</v>
+      </c>
+      <c r="E35" s="2">
+        <v>10</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="2">
+        <v>1698</v>
+      </c>
+      <c r="B36" s="2">
+        <v>191</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+      <c r="D36" s="2">
+        <v>7</v>
+      </c>
+      <c r="E36" s="2">
+        <v>13</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="2">
+        <v>1738</v>
+      </c>
+      <c r="B37" s="2">
+        <v>40</v>
+      </c>
+      <c r="C37" s="2">
+        <v>3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>7</v>
+      </c>
+      <c r="E37" s="2">
+        <v>7</v>
+      </c>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="F38"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G38">
+    <sortCondition ref="A2:A38"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44F401D-6AED-436F-A0B9-E4B3B95A5FFC}">
   <sheetPr>
@@ -3195,7 +3905,7 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32:F37"/>
     </sheetView>
   </sheetViews>
@@ -4614,8 +5324,8 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:F37"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6033,9 +6743,9 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6747,8 +7457,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010094AA1C2EC61FF14F854275BACE97F8DB" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="87e5dad36149ef9875866ee6c07b51c0">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="a7d62638-28e2-4f67-9303-2f0acda7ac7b" xmlns:ns4="5c7bd4c1-27c7-4857-97c5-5e05b5492f18" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b71da207586abf436948836a167800a" ns1:_="" ns3:_="" ns4:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="a7d62638-28e2-4f67-9303-2f0acda7ac7b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010094AA1C2EC61FF14F854275BACE97F8DB" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7ed8f1bbf957748ffc396fce8d8e9def">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="a7d62638-28e2-4f67-9303-2f0acda7ac7b" xmlns:ns4="5c7bd4c1-27c7-4857-97c5-5e05b5492f18" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ada7cf4f373b2b21e20b3c9d8b6ea551" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="a7d62638-28e2-4f67-9303-2f0acda7ac7b"/>
     <xsd:import namespace="5c7bd4c1-27c7-4857-97c5-5e05b5492f18"/>
@@ -6774,6 +7503,8 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6853,6 +7584,16 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="24" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="25" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -6992,26 +7733,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3314082-2A5E-4500-BC8F-959EA6E2438F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{496C6FD6-E5A0-4368-8492-A4784BEDD3E5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7019,5 +7742,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{496C6FD6-E5A0-4368-8492-A4784BEDD3E5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{432F2062-72EA-4E1E-99E3-A44A38B68525}"/>
 </file>
</xml_diff>

<commit_message>
Add new sessions and utilities for testing pipelines.
This should also make it easier to add new sessions in the future.
</commit_message>
<xml_diff>
--- a/data/01_raw/2023_ground_truth_counts.xlsx
+++ b/data/01_raw/2023_ground_truth_counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26821"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26903"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/dawest_uga_edu/Documents/Documents/UGA Grad School/Masters Research/PTs Drone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawest\OneDrive - University of Georgia\Documents\UGA Grad School\Masters Research\PTs Drone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABA7B3B8-0205-42DC-9FC6-46E91AAE057E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{498252B1-763C-4C8E-A72F-8C23CED42BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="9" activeTab="9" xr2:uid="{8F9DACAF-C196-4FF0-BBE7-23C747EA27F6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="11" activeTab="11" xr2:uid="{8F9DACAF-C196-4FF0-BBE7-23C747EA27F6}"/>
   </bookViews>
   <sheets>
     <sheet name="7-27-23" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="8-21-23" sheetId="8" r:id="rId8"/>
     <sheet name="8-24-23" sheetId="9" r:id="rId9"/>
     <sheet name="8-28-23" sheetId="10" r:id="rId10"/>
+    <sheet name="9-1-23" sheetId="11" r:id="rId11"/>
+    <sheet name="9-5-23" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="13">
   <si>
     <t>Plot</t>
   </si>
@@ -149,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -160,6 +162,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1070,8 +1075,8 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1762,6 +1767,1418 @@
     </row>
     <row r="38" spans="1:6">
       <c r="F38"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G38">
+    <sortCondition ref="A2:A38"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871F9791-F576-4C67-8010-BDBE929CF2D4}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="8" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="19.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="2">
+        <v>1007</v>
+      </c>
+      <c r="B2" s="2">
+        <v>169</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="2">
+        <v>1051</v>
+      </c>
+      <c r="B3" s="2">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="2">
+        <v>1055</v>
+      </c>
+      <c r="B4" s="2">
+        <v>134</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="2">
+        <v>1057</v>
+      </c>
+      <c r="B5" s="2">
+        <v>107</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="2">
+        <v>1069</v>
+      </c>
+      <c r="B6" s="2">
+        <v>104</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="2">
+        <v>1078</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="2">
+        <v>1085</v>
+      </c>
+      <c r="B8" s="2">
+        <v>147</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="2">
+        <v>1092</v>
+      </c>
+      <c r="B9" s="2">
+        <v>204</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="2">
+        <v>1119</v>
+      </c>
+      <c r="B10" s="2">
+        <v>158</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="2">
+        <v>1132</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="2">
+        <v>1135</v>
+      </c>
+      <c r="B12" s="2">
+        <v>162</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="2">
+        <v>1237</v>
+      </c>
+      <c r="B13" s="2">
+        <v>210</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="2">
+        <v>1301</v>
+      </c>
+      <c r="B14" s="2">
+        <v>204</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="2">
+        <v>1313</v>
+      </c>
+      <c r="B15" s="2">
+        <v>104</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="2">
+        <v>1349</v>
+      </c>
+      <c r="B16" s="2">
+        <v>158</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="2">
+        <v>1382</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="2">
+        <v>1417</v>
+      </c>
+      <c r="B18" s="2">
+        <v>107</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>4</v>
+      </c>
+      <c r="E18" s="2">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="2">
+        <v>1419</v>
+      </c>
+      <c r="B19" s="2">
+        <v>210</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>15</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="2">
+        <v>1437</v>
+      </c>
+      <c r="B20" s="2">
+        <v>147</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="2">
+        <v>1444</v>
+      </c>
+      <c r="B21" s="2">
+        <v>162</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>11</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="2">
+        <v>1464</v>
+      </c>
+      <c r="B22" s="2">
+        <v>169</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="2">
+        <v>1469</v>
+      </c>
+      <c r="B23" s="2">
+        <v>134</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>13</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="2">
+        <v>1485</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>15</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="2">
+        <v>1509</v>
+      </c>
+      <c r="B25" s="2">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2">
+        <v>13</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A26" s="2">
+        <v>1536</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>10</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A27" s="2">
+        <v>1544</v>
+      </c>
+      <c r="B27" s="2">
+        <v>169</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>14</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="2">
+        <v>1550</v>
+      </c>
+      <c r="B28" s="2">
+        <v>158</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="2">
+        <v>1551</v>
+      </c>
+      <c r="B29" s="2">
+        <v>104</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>9</v>
+      </c>
+      <c r="E29" s="2">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A30" s="2">
+        <v>1563</v>
+      </c>
+      <c r="B30" s="2">
+        <v>162</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+      <c r="D30" s="2">
+        <v>3</v>
+      </c>
+      <c r="E30" s="2">
+        <v>9</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="2">
+        <v>1571</v>
+      </c>
+      <c r="B31" s="2">
+        <v>107</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="2">
+        <v>1612</v>
+      </c>
+      <c r="B32" s="2">
+        <v>14</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="2">
+        <v>6</v>
+      </c>
+      <c r="E32" s="2">
+        <v>10</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="2">
+        <v>1621</v>
+      </c>
+      <c r="B33" s="2">
+        <v>204</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2">
+        <v>10</v>
+      </c>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="2">
+        <v>1641</v>
+      </c>
+      <c r="B34" s="2">
+        <v>134</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2">
+        <v>9</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A35" s="2">
+        <v>1676</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2">
+        <v>14</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="2">
+        <v>1711</v>
+      </c>
+      <c r="B36" s="2">
+        <v>147</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>8</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="2">
+        <v>1748</v>
+      </c>
+      <c r="B37" s="2">
+        <v>210</v>
+      </c>
+      <c r="C37" s="2">
+        <v>3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2">
+        <v>13</v>
+      </c>
+      <c r="F37" s="2"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G38">
+    <sortCondition ref="A2:A38"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36F1322-7A8E-41E1-9C0D-8367F4BDCBF6}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="8" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="19.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5">
+        <v>45174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="2">
+        <v>1078</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="2">
+        <v>1131</v>
+      </c>
+      <c r="B3" s="2">
+        <v>152</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="2">
+        <v>1132</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="2">
+        <v>1133</v>
+      </c>
+      <c r="B5" s="2">
+        <v>80</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="2">
+        <v>1139</v>
+      </c>
+      <c r="B6" s="2">
+        <v>230</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="2">
+        <v>1147</v>
+      </c>
+      <c r="B7" s="2">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="2">
+        <v>1164</v>
+      </c>
+      <c r="B8" s="2">
+        <v>98</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="2">
+        <v>1195</v>
+      </c>
+      <c r="B9" s="2">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="2">
+        <v>1240</v>
+      </c>
+      <c r="B10" s="2">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="2">
+        <v>1249</v>
+      </c>
+      <c r="B11" s="2">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="2">
+        <v>1252</v>
+      </c>
+      <c r="B12" s="2">
+        <v>141</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="2">
+        <v>1256</v>
+      </c>
+      <c r="B13" s="2">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>7</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="2">
+        <v>1261</v>
+      </c>
+      <c r="B14" s="2">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="2">
+        <v>1269</v>
+      </c>
+      <c r="B15" s="2">
+        <v>80</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="2">
+        <v>1354</v>
+      </c>
+      <c r="B16" s="2">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>7</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="2">
+        <v>1362</v>
+      </c>
+      <c r="B17" s="2">
+        <v>230</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>14</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="2">
+        <v>1379</v>
+      </c>
+      <c r="B18" s="2">
+        <v>98</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>15</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="2">
+        <v>1382</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>8</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="2">
+        <v>1391</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="2">
+        <v>1403</v>
+      </c>
+      <c r="B21" s="2">
+        <v>152</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="2">
+        <v>1423</v>
+      </c>
+      <c r="B22" s="2">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>7</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="2">
+        <v>1477</v>
+      </c>
+      <c r="B23" s="2">
+        <v>141</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="2">
+        <v>1485</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="2">
+        <v>1492</v>
+      </c>
+      <c r="B25" s="2">
+        <v>50</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>9</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A26" s="2">
+        <v>1534</v>
+      </c>
+      <c r="B26" s="2">
+        <v>80</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A27" s="2">
+        <v>1536</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>10</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="2">
+        <v>1577</v>
+      </c>
+      <c r="B28" s="2">
+        <v>44</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>9</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="2">
+        <v>1595</v>
+      </c>
+      <c r="B29" s="2">
+        <v>230</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>3</v>
+      </c>
+      <c r="E29" s="2">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A30" s="2">
+        <v>1611</v>
+      </c>
+      <c r="B30" s="2">
+        <v>152</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>8</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="2">
+        <v>1653</v>
+      </c>
+      <c r="B31" s="2">
+        <v>25</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
+      <c r="D31" s="2">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="2">
+        <v>1663</v>
+      </c>
+      <c r="B32" s="2">
+        <v>31</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3</v>
+      </c>
+      <c r="E32" s="2">
+        <v>8</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="2">
+        <v>1676</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2">
+        <v>12</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="2">
+        <v>1681</v>
+      </c>
+      <c r="B34" s="2">
+        <v>50</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
+        <v>11</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A35" s="2">
+        <v>1685</v>
+      </c>
+      <c r="B35" s="2">
+        <v>141</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>3</v>
+      </c>
+      <c r="E35" s="2">
+        <v>10</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="2">
+        <v>1712</v>
+      </c>
+      <c r="B36" s="2">
+        <v>98</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2">
+        <v>11</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="2">
+        <v>1738</v>
+      </c>
+      <c r="B37" s="2">
+        <v>40</v>
+      </c>
+      <c r="C37" s="2">
+        <v>3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+      <c r="E37" s="2">
+        <v>8</v>
+      </c>
+      <c r="F37" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G38">
@@ -6744,7 +8161,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -7457,16 +8874,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_activity xmlns="a7d62638-28e2-4f67-9303-2f0acda7ac7b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -7475,7 +8882,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010094AA1C2EC61FF14F854275BACE97F8DB" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7ed8f1bbf957748ffc396fce8d8e9def">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="a7d62638-28e2-4f67-9303-2f0acda7ac7b" xmlns:ns4="5c7bd4c1-27c7-4857-97c5-5e05b5492f18" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ada7cf4f373b2b21e20b3c9d8b6ea551" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7733,14 +9140,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="a7d62638-28e2-4f67-9303-2f0acda7ac7b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{496C6FD6-E5A0-4368-8492-A4784BEDD3E5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD7C944F-C3D4-460D-AE36-4D3A5F868739}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD7C944F-C3D4-460D-AE36-4D3A5F868739}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{432F2062-72EA-4E1E-99E3-A44A38B68525}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{432F2062-72EA-4E1E-99E3-A44A38B68525}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{496C6FD6-E5A0-4368-8492-A4784BEDD3E5}"/>
 </file>
</xml_diff>